<commit_message>
OCEPROJECT-4609: Testing Page Options and Page Options buttons.
</commit_message>
<xml_diff>
--- a/test-data/page-options.xlsx
+++ b/test-data/page-options.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\WCMS\TestSuite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69D4A2D6-3EBF-4DF3-A892-01D2FA5DD355}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5E2D8B7-85B4-4975-80D6-6F62A9EB4E50}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21060" windowHeight="12540" xr2:uid="{EFF3C207-6FC0-4D04-84EF-45DB1C2E8D27}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21060" windowHeight="12540" activeTab="1" xr2:uid="{EFF3C207-6FC0-4D04-84EF-45DB1C2E8D27}"/>
   </bookViews>
   <sheets>
-    <sheet name="Visible Page Options" sheetId="1" r:id="rId1"/>
-    <sheet name="Not Visible Page Options" sheetId="2" r:id="rId2"/>
+    <sheet name="All Pages" sheetId="3" r:id="rId1"/>
+    <sheet name="Visible Page Options" sheetId="1" r:id="rId2"/>
+    <sheet name="Not Visible Page Options" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="28">
   <si>
     <t>PageOptions Link</t>
   </si>
@@ -469,11 +470,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C345D6C-DF3E-47DC-B08A-E822CBA15E43}">
-  <dimension ref="A1:K6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3929A153-EBA0-496E-BFE7-A29B331AEF00}">
+  <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -547,22 +548,22 @@
       <c r="D3" t="s">
         <v>3</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>8</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>9</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>10</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>11</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>12</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>13</v>
       </c>
     </row>
@@ -579,10 +580,10 @@
       <c r="D4" t="s">
         <v>5</v>
       </c>
-      <c r="E4" t="s">
+      <c r="G4" t="s">
         <v>9</v>
       </c>
-      <c r="F4" t="s">
+      <c r="I4" t="s">
         <v>11</v>
       </c>
     </row>
@@ -634,22 +635,240 @@
       <c r="D6" t="s">
         <v>3</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>8</v>
       </c>
+      <c r="G6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" t="s">
+        <v>11</v>
+      </c>
+      <c r="J6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C345D6C-DF3E-47DC-B08A-E822CBA15E43}">
+  <dimension ref="A1:K6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.7109375" customWidth="1"/>
+    <col min="2" max="2" width="48.28515625" customWidth="1"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
+    <col min="4" max="4" width="30.28515625" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
       <c r="F6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" t="s">
         <v>9</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>10</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>11</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>12</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>13</v>
       </c>
     </row>
@@ -659,12 +878,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3C5DDC6-63D8-46D9-AC4D-F73BC5AAF5EE}">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A2" sqref="A2:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update page options spreadsheet
</commit_message>
<xml_diff>
--- a/test-data/page-options.xlsx
+++ b/test-data/page-options.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\WCMS\TestSuite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5E2D8B7-85B4-4975-80D6-6F62A9EB4E50}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DACA39F9-37B2-4B47-8681-8F185937618B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21060" windowHeight="12540" activeTab="1" xr2:uid="{EFF3C207-6FC0-4D04-84EF-45DB1C2E8D27}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21060" windowHeight="12540" xr2:uid="{EFF3C207-6FC0-4D04-84EF-45DB1C2E8D27}"/>
   </bookViews>
   <sheets>
     <sheet name="All Pages" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="60">
   <si>
     <t>PageOptions Link</t>
   </si>
@@ -111,6 +111,102 @@
   </si>
   <si>
     <t>/espanol/cancer</t>
+  </si>
+  <si>
+    <t>font</t>
+  </si>
+  <si>
+    <t>bottom buttons</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>/about-cancer/treatment/clinical-trials/search</t>
+  </si>
+  <si>
+    <t>/publications/dictionaries/cancer-terms</t>
+  </si>
+  <si>
+    <t>No font resizer on App Module Pages</t>
+  </si>
+  <si>
+    <t>/about-cancer/treatment/clinical-trials/advanced-search</t>
+  </si>
+  <si>
+    <t>/about-cancer/causes-prevention/genetics/directory</t>
+  </si>
+  <si>
+    <t>/about-cancer/causes-prevention/genetics/directory/results</t>
+  </si>
+  <si>
+    <t>/about-cancer/causes-prevention/genetics/directory/view</t>
+  </si>
+  <si>
+    <t>/about-cancer/treatment/clinical-trials/search/r</t>
+  </si>
+  <si>
+    <t>/about-cancer/treatment/clinical-trials/search/v</t>
+  </si>
+  <si>
+    <t>/about-cancer/treatment/clinical-trials/disease</t>
+  </si>
+  <si>
+    <t>/about-cancer/treatment/clinical-trials/intervention</t>
+  </si>
+  <si>
+    <t>/about-cancer/treatment/clinical-trials/transitional-cell-cancer-renal-pelvis-ureter</t>
+  </si>
+  <si>
+    <t>/about-cancer/treatment/clinical-trials/kidney-cancer</t>
+  </si>
+  <si>
+    <t>/about-cancer/treatment/clinical-trials/testicular-cancer</t>
+  </si>
+  <si>
+    <t>/about-cancer/treatment/clinical-trials/adult-brain-tumors</t>
+  </si>
+  <si>
+    <t>/about-cancer/treatment/clinical-trials/adult-glioblastoma</t>
+  </si>
+  <si>
+    <t>/about-cancer/treatment/clinical-trials/adult-metastatic-brain-tumors</t>
+  </si>
+  <si>
+    <t>/about-cancer/treatment/clinical-trials/childhood-astrocytoma</t>
+  </si>
+  <si>
+    <t>/about-cancer/treatment/clinical-trials/childhood-embryonal-tumors</t>
+  </si>
+  <si>
+    <t>/about-cancer/treatment/clinical-trials/childhood-brainstem-glioma</t>
+  </si>
+  <si>
+    <t>/about-cancer/treatment/clinical-trials/pituitary-tumors</t>
+  </si>
+  <si>
+    <t>/nci/rare-brain-spine-tumor/nci-connection-search-results</t>
+  </si>
+  <si>
+    <t>/about-cancer/treatment/clinical-trials/thymoma-thymic-carcinoma</t>
+  </si>
+  <si>
+    <t>/search/results</t>
+  </si>
+  <si>
+    <t>/espanol/buscar/resultados</t>
+  </si>
+  <si>
+    <t>/espanol/publicaciones/diccionario</t>
+  </si>
+  <si>
+    <t>/publications/dictionaries/cancer-drug</t>
+  </si>
+  <si>
+    <t>/publications/dictionaries/genetics-dictionary</t>
+  </si>
+  <si>
+    <t>/sites/nano/nan</t>
   </si>
 </sst>
 </file>
@@ -154,9 +250,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -471,19 +568,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3929A153-EBA0-496E-BFE7-A29B331AEF00}">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.7109375" customWidth="1"/>
-    <col min="2" max="2" width="48.28515625" customWidth="1"/>
-    <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="30.28515625" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="41" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" customWidth="1"/>
+    <col min="11" max="11" width="52.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -497,6 +594,27 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -511,28 +629,28 @@
         <v>17</v>
       </c>
       <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" t="s">
         <v>16</v>
-      </c>
-      <c r="E2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" t="s">
-        <v>11</v>
-      </c>
-      <c r="J2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -540,31 +658,34 @@
         <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>3</v>
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>30</v>
       </c>
       <c r="F3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H3" t="s">
         <v>10</v>
       </c>
       <c r="I3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="K3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -572,19 +693,31 @@
         <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
       </c>
       <c r="G4" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="H4" t="s">
+        <v>10</v>
       </c>
       <c r="I4" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="J4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K4" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -592,34 +725,31 @@
         <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="F5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H5" t="s">
         <v>10</v>
       </c>
       <c r="I5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="K5" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -627,31 +757,19 @@
         <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="E6" t="s">
+        <v>30</v>
       </c>
       <c r="F6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6" t="s">
-        <v>10</v>
-      </c>
-      <c r="I6" t="s">
-        <v>11</v>
-      </c>
-      <c r="J6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K6" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -664,7 +782,7 @@
       <c r="C7" t="s">
         <v>6</v>
       </c>
-      <c r="D7" t="s">
+      <c r="K7" t="s">
         <v>15</v>
       </c>
     </row>
@@ -678,12 +796,973 @@
       <c r="C8" t="s">
         <v>6</v>
       </c>
-      <c r="D8" t="s">
+      <c r="K8" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" t="s">
+        <v>10</v>
+      </c>
+      <c r="I9" t="s">
+        <v>12</v>
+      </c>
+      <c r="J9" t="s">
+        <v>13</v>
+      </c>
+      <c r="K9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" t="s">
+        <v>10</v>
+      </c>
+      <c r="I10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J10" t="s">
+        <v>13</v>
+      </c>
+      <c r="K10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H11" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" t="s">
+        <v>12</v>
+      </c>
+      <c r="J11" t="s">
+        <v>13</v>
+      </c>
+      <c r="K11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" t="s">
+        <v>8</v>
+      </c>
+      <c r="H12" t="s">
+        <v>10</v>
+      </c>
+      <c r="I12" t="s">
+        <v>12</v>
+      </c>
+      <c r="J12" t="s">
+        <v>13</v>
+      </c>
+      <c r="K12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" t="s">
+        <v>8</v>
+      </c>
+      <c r="H13" t="s">
+        <v>10</v>
+      </c>
+      <c r="I13" t="s">
+        <v>12</v>
+      </c>
+      <c r="J13" t="s">
+        <v>13</v>
+      </c>
+      <c r="K13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" t="s">
+        <v>30</v>
+      </c>
+      <c r="F14" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I14" t="s">
+        <v>12</v>
+      </c>
+      <c r="J14" t="s">
+        <v>13</v>
+      </c>
+      <c r="K14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" t="s">
+        <v>8</v>
+      </c>
+      <c r="H15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I15" t="s">
+        <v>12</v>
+      </c>
+      <c r="J15" t="s">
+        <v>13</v>
+      </c>
+      <c r="K15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" t="s">
+        <v>30</v>
+      </c>
+      <c r="F16" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16" t="s">
+        <v>8</v>
+      </c>
+      <c r="H16" t="s">
+        <v>10</v>
+      </c>
+      <c r="I16" t="s">
+        <v>12</v>
+      </c>
+      <c r="J16" t="s">
+        <v>13</v>
+      </c>
+      <c r="K16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" t="s">
+        <v>30</v>
+      </c>
+      <c r="F17" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17" t="s">
+        <v>8</v>
+      </c>
+      <c r="H17" t="s">
+        <v>10</v>
+      </c>
+      <c r="I17" t="s">
+        <v>12</v>
+      </c>
+      <c r="J17" t="s">
+        <v>13</v>
+      </c>
+      <c r="K17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" t="s">
+        <v>30</v>
+      </c>
+      <c r="F18" t="s">
+        <v>11</v>
+      </c>
+      <c r="G18" t="s">
+        <v>8</v>
+      </c>
+      <c r="H18" t="s">
+        <v>10</v>
+      </c>
+      <c r="I18" t="s">
+        <v>12</v>
+      </c>
+      <c r="J18" t="s">
+        <v>13</v>
+      </c>
+      <c r="K18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" t="s">
+        <v>30</v>
+      </c>
+      <c r="F19" t="s">
+        <v>11</v>
+      </c>
+      <c r="G19" t="s">
+        <v>8</v>
+      </c>
+      <c r="H19" t="s">
+        <v>10</v>
+      </c>
+      <c r="I19" t="s">
+        <v>12</v>
+      </c>
+      <c r="J19" t="s">
+        <v>13</v>
+      </c>
+      <c r="K19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" t="s">
+        <v>30</v>
+      </c>
+      <c r="F20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G20" t="s">
+        <v>8</v>
+      </c>
+      <c r="H20" t="s">
+        <v>10</v>
+      </c>
+      <c r="I20" t="s">
+        <v>12</v>
+      </c>
+      <c r="J20" t="s">
+        <v>13</v>
+      </c>
+      <c r="K20" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" t="s">
+        <v>30</v>
+      </c>
+      <c r="F21" t="s">
+        <v>11</v>
+      </c>
+      <c r="G21" t="s">
+        <v>8</v>
+      </c>
+      <c r="H21" t="s">
+        <v>10</v>
+      </c>
+      <c r="I21" t="s">
+        <v>12</v>
+      </c>
+      <c r="J21" t="s">
+        <v>13</v>
+      </c>
+      <c r="K21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" t="s">
+        <v>30</v>
+      </c>
+      <c r="F22" t="s">
+        <v>11</v>
+      </c>
+      <c r="G22" t="s">
+        <v>8</v>
+      </c>
+      <c r="H22" t="s">
+        <v>10</v>
+      </c>
+      <c r="I22" t="s">
+        <v>12</v>
+      </c>
+      <c r="J22" t="s">
+        <v>13</v>
+      </c>
+      <c r="K22" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" t="s">
+        <v>30</v>
+      </c>
+      <c r="F23" t="s">
+        <v>11</v>
+      </c>
+      <c r="G23" t="s">
+        <v>8</v>
+      </c>
+      <c r="H23" t="s">
+        <v>10</v>
+      </c>
+      <c r="I23" t="s">
+        <v>12</v>
+      </c>
+      <c r="J23" t="s">
+        <v>13</v>
+      </c>
+      <c r="K23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" t="s">
+        <v>30</v>
+      </c>
+      <c r="F24" t="s">
+        <v>11</v>
+      </c>
+      <c r="G24" t="s">
+        <v>8</v>
+      </c>
+      <c r="H24" t="s">
+        <v>10</v>
+      </c>
+      <c r="I24" t="s">
+        <v>12</v>
+      </c>
+      <c r="J24" t="s">
+        <v>13</v>
+      </c>
+      <c r="K24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25" t="s">
+        <v>47</v>
+      </c>
+      <c r="C25" t="s">
+        <v>7</v>
+      </c>
+      <c r="E25" t="s">
+        <v>30</v>
+      </c>
+      <c r="F25" t="s">
+        <v>11</v>
+      </c>
+      <c r="G25" t="s">
+        <v>8</v>
+      </c>
+      <c r="H25" t="s">
+        <v>10</v>
+      </c>
+      <c r="I25" t="s">
+        <v>12</v>
+      </c>
+      <c r="J25" t="s">
+        <v>13</v>
+      </c>
+      <c r="K25" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E26" t="s">
+        <v>30</v>
+      </c>
+      <c r="F26" t="s">
+        <v>11</v>
+      </c>
+      <c r="G26" t="s">
+        <v>8</v>
+      </c>
+      <c r="H26" t="s">
+        <v>10</v>
+      </c>
+      <c r="I26" t="s">
+        <v>12</v>
+      </c>
+      <c r="J26" t="s">
+        <v>13</v>
+      </c>
+      <c r="K26" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" t="s">
+        <v>49</v>
+      </c>
+      <c r="C27" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" t="s">
+        <v>30</v>
+      </c>
+      <c r="F27" t="s">
+        <v>11</v>
+      </c>
+      <c r="G27" t="s">
+        <v>8</v>
+      </c>
+      <c r="H27" t="s">
+        <v>10</v>
+      </c>
+      <c r="I27" t="s">
+        <v>12</v>
+      </c>
+      <c r="J27" t="s">
+        <v>13</v>
+      </c>
+      <c r="K27" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>19</v>
+      </c>
+      <c r="B28" t="s">
+        <v>50</v>
+      </c>
+      <c r="C28" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" t="s">
+        <v>30</v>
+      </c>
+      <c r="F28" t="s">
+        <v>11</v>
+      </c>
+      <c r="G28" t="s">
+        <v>8</v>
+      </c>
+      <c r="H28" t="s">
+        <v>10</v>
+      </c>
+      <c r="I28" t="s">
+        <v>12</v>
+      </c>
+      <c r="J28" t="s">
+        <v>13</v>
+      </c>
+      <c r="K28" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B29" t="s">
+        <v>51</v>
+      </c>
+      <c r="C29" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" t="s">
+        <v>30</v>
+      </c>
+      <c r="F29" t="s">
+        <v>11</v>
+      </c>
+      <c r="G29" t="s">
+        <v>8</v>
+      </c>
+      <c r="H29" t="s">
+        <v>10</v>
+      </c>
+      <c r="I29" t="s">
+        <v>12</v>
+      </c>
+      <c r="J29" t="s">
+        <v>13</v>
+      </c>
+      <c r="K29" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>19</v>
+      </c>
+      <c r="B30" t="s">
+        <v>52</v>
+      </c>
+      <c r="C30" t="s">
+        <v>7</v>
+      </c>
+      <c r="E30" t="s">
+        <v>30</v>
+      </c>
+      <c r="F30" t="s">
+        <v>11</v>
+      </c>
+      <c r="G30" t="s">
+        <v>8</v>
+      </c>
+      <c r="H30" t="s">
+        <v>10</v>
+      </c>
+      <c r="I30" t="s">
+        <v>12</v>
+      </c>
+      <c r="J30" t="s">
+        <v>13</v>
+      </c>
+      <c r="K30" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B31" t="s">
+        <v>53</v>
+      </c>
+      <c r="C31" t="s">
+        <v>7</v>
+      </c>
+      <c r="E31" t="s">
+        <v>30</v>
+      </c>
+      <c r="F31" t="s">
+        <v>11</v>
+      </c>
+      <c r="G31" t="s">
+        <v>8</v>
+      </c>
+      <c r="H31" t="s">
+        <v>10</v>
+      </c>
+      <c r="I31" t="s">
+        <v>12</v>
+      </c>
+      <c r="J31" t="s">
+        <v>13</v>
+      </c>
+      <c r="K31" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>19</v>
+      </c>
+      <c r="B32" t="s">
+        <v>54</v>
+      </c>
+      <c r="C32" t="s">
+        <v>7</v>
+      </c>
+      <c r="E32" t="s">
+        <v>30</v>
+      </c>
+      <c r="F32" t="s">
+        <v>11</v>
+      </c>
+      <c r="G32" t="s">
+        <v>8</v>
+      </c>
+      <c r="H32" t="s">
+        <v>10</v>
+      </c>
+      <c r="I32" t="s">
+        <v>12</v>
+      </c>
+      <c r="J32" t="s">
+        <v>13</v>
+      </c>
+      <c r="K32" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33" t="s">
+        <v>55</v>
+      </c>
+      <c r="C33" t="s">
+        <v>7</v>
+      </c>
+      <c r="E33" t="s">
+        <v>30</v>
+      </c>
+      <c r="F33" t="s">
+        <v>11</v>
+      </c>
+      <c r="G33" t="s">
+        <v>8</v>
+      </c>
+      <c r="H33" t="s">
+        <v>10</v>
+      </c>
+      <c r="I33" t="s">
+        <v>12</v>
+      </c>
+      <c r="J33" t="s">
+        <v>13</v>
+      </c>
+      <c r="K33" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B34" t="s">
+        <v>32</v>
+      </c>
+      <c r="C34" t="s">
+        <v>7</v>
+      </c>
+      <c r="E34" t="s">
+        <v>30</v>
+      </c>
+      <c r="F34" t="s">
+        <v>11</v>
+      </c>
+      <c r="G34" t="s">
+        <v>8</v>
+      </c>
+      <c r="H34" t="s">
+        <v>10</v>
+      </c>
+      <c r="I34" t="s">
+        <v>12</v>
+      </c>
+      <c r="J34" t="s">
+        <v>13</v>
+      </c>
+      <c r="K34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>19</v>
+      </c>
+      <c r="B35" t="s">
+        <v>56</v>
+      </c>
+      <c r="C35" t="s">
+        <v>7</v>
+      </c>
+      <c r="E35" t="s">
+        <v>30</v>
+      </c>
+      <c r="F35" t="s">
+        <v>11</v>
+      </c>
+      <c r="G35" t="s">
+        <v>8</v>
+      </c>
+      <c r="H35" t="s">
+        <v>10</v>
+      </c>
+      <c r="I35" t="s">
+        <v>12</v>
+      </c>
+      <c r="J35" t="s">
+        <v>13</v>
+      </c>
+      <c r="K35" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B36" t="s">
+        <v>57</v>
+      </c>
+      <c r="C36" t="s">
+        <v>7</v>
+      </c>
+      <c r="E36" t="s">
+        <v>30</v>
+      </c>
+      <c r="F36" t="s">
+        <v>11</v>
+      </c>
+      <c r="G36" t="s">
+        <v>8</v>
+      </c>
+      <c r="H36" t="s">
+        <v>10</v>
+      </c>
+      <c r="I36" t="s">
+        <v>12</v>
+      </c>
+      <c r="J36" t="s">
+        <v>13</v>
+      </c>
+      <c r="K36" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>19</v>
+      </c>
+      <c r="B37" t="s">
+        <v>58</v>
+      </c>
+      <c r="C37" t="s">
+        <v>7</v>
+      </c>
+      <c r="E37" t="s">
+        <v>30</v>
+      </c>
+      <c r="F37" t="s">
+        <v>11</v>
+      </c>
+      <c r="G37" t="s">
+        <v>8</v>
+      </c>
+      <c r="H37" t="s">
+        <v>10</v>
+      </c>
+      <c r="I37" t="s">
+        <v>12</v>
+      </c>
+      <c r="J37" t="s">
+        <v>13</v>
+      </c>
+      <c r="K37" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B38" t="s">
+        <v>59</v>
+      </c>
+      <c r="C38" t="s">
+        <v>7</v>
+      </c>
+      <c r="E38" t="s">
+        <v>30</v>
+      </c>
+      <c r="F38" t="s">
+        <v>11</v>
+      </c>
+      <c r="G38" t="s">
+        <v>8</v>
+      </c>
+      <c r="H38" t="s">
+        <v>10</v>
+      </c>
+      <c r="I38" t="s">
+        <v>12</v>
+      </c>
+      <c r="J38" t="s">
+        <v>13</v>
+      </c>
+      <c r="K38" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -691,7 +1770,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C345D6C-DF3E-47DC-B08A-E822CBA15E43}">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Removed links linking to Page Not Found.  Added test for AZList.
</commit_message>
<xml_diff>
--- a/test-data/page-options.xlsx
+++ b/test-data/page-options.xlsx
@@ -8,14 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\WCMS\TestSuite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{03313ADF-17D5-4992-A16E-8F0472F22ACA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{0A981B91-FE30-44FC-8760-C5C3D3F856E8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21060" windowHeight="12540" xr2:uid="{EFF3C207-6FC0-4D04-84EF-45DB1C2E8D27}"/>
   </bookViews>
   <sheets>
     <sheet name="All Pages" sheetId="3" r:id="rId1"/>
-    <sheet name="Visible Page Options" sheetId="1" r:id="rId2"/>
-    <sheet name="Not Visible Page Options" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -27,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="51">
   <si>
     <t>PageOptions Link</t>
   </si>
@@ -44,9 +42,6 @@
     <t>r4r</t>
   </si>
   <si>
-    <t>bottom button</t>
-  </si>
-  <si>
     <t>none</t>
   </si>
   <si>
@@ -56,9 +51,6 @@
     <t>print</t>
   </si>
   <si>
-    <t>mail</t>
-  </si>
-  <si>
     <t>facebook</t>
   </si>
   <si>
@@ -74,39 +66,21 @@
     <t>FontResize</t>
   </si>
   <si>
-    <t>no buttons, CTS print pages, dictionary pop-ups, livehelp</t>
-  </si>
-  <si>
     <t>all buttons, Content pages, article, factsheet, topic page, press release, institution, cancer research page, general page, pdq summaries, blog posts, blog series</t>
   </si>
   <si>
     <t>all</t>
   </si>
   <si>
-    <t>Hostname</t>
-  </si>
-  <si>
-    <t>https://www-qa.cancer.gov</t>
-  </si>
-  <si>
     <t>/about-cancer/understanding/what-is-cancer</t>
   </si>
   <si>
     <t>/about-cancer</t>
   </si>
   <si>
-    <t>/</t>
-  </si>
-  <si>
-    <t>https://livehelp.cancer.gov</t>
-  </si>
-  <si>
     <t>/research/resources</t>
   </si>
   <si>
-    <t>https://livehelp-es.cancer.gov</t>
-  </si>
-  <si>
     <t>/espanol/cancer/naturaleza/que-es</t>
   </si>
   <si>
@@ -146,15 +120,6 @@
     <t>/about-cancer/treatment/clinical-trials/search/r</t>
   </si>
   <si>
-    <t>/about-cancer/treatment/clinical-trials/search/v</t>
-  </si>
-  <si>
-    <t>/about-cancer/treatment/clinical-trials/disease</t>
-  </si>
-  <si>
-    <t>/about-cancer/treatment/clinical-trials/intervention</t>
-  </si>
-  <si>
     <t>/about-cancer/treatment/clinical-trials/transitional-cell-cancer-renal-pelvis-ureter</t>
   </si>
   <si>
@@ -185,12 +150,6 @@
     <t>/about-cancer/treatment/clinical-trials/pituitary-tumors</t>
   </si>
   <si>
-    <t>/nci/rare-brain-spine-tumor/nci-connection-search-results</t>
-  </si>
-  <si>
-    <t>/about-cancer/treatment/clinical-trials/thymoma-thymic-carcinoma</t>
-  </si>
-  <si>
     <t>/search/results</t>
   </si>
   <si>
@@ -206,19 +165,19 @@
     <t>/publications/dictionaries/genetics-dictionary</t>
   </si>
   <si>
-    <t>/sites/nano/nan</t>
-  </si>
-  <si>
     <t>/about-cancer/treatment/clinical-trials/search/foobar</t>
   </si>
   <si>
     <t>Page Not Found page</t>
   </si>
   <si>
-    <t>??? Page not found</t>
-  </si>
-  <si>
     <t xml:space="preserve">default buttons </t>
+  </si>
+  <si>
+    <t>/about-cancer/treatment/clinical-trials/search/v?loc=0&amp;rl=1&amp;id=NCI-2015-01918&amp;pn=1&amp;ni=10</t>
+  </si>
+  <si>
+    <t>/sites/nano</t>
   </si>
 </sst>
 </file>
@@ -580,10 +539,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3929A153-EBA0-496E-BFE7-A29B331AEF00}">
-  <dimension ref="A1:J37"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -602,25 +561,25 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>2</v>
@@ -628,121 +587,121 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" t="s">
         <v>13</v>
-      </c>
-      <c r="J2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" t="s">
         <v>13</v>
-      </c>
-      <c r="J3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J4" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="E5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J5" t="s">
         <v>3</v>
@@ -750,1159 +709,785 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="E6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="J6" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="E7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J7" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="E8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J8" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D9" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="E9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J9" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="E10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J10" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D11" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="E11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G11" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I11" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J11" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B12" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D12" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="E12" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G12" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I12" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J12" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B13" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D13" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="E13" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G13" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H13" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I13" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J13" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B14" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D14" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="E14" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G14" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H14" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I14" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J14" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="B15" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="E15" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G15" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H15" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I15" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J15" t="s">
-        <v>62</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="B16" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D16" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="E16" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G16" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H16" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I16" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J16" t="s">
-        <v>62</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="B17" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D17" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="E17" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H17" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I17" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J17" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B18" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D18" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="E18" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G18" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H18" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I18" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J18" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="B19" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D19" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="E19" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G19" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H19" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I19" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J19" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="B20" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D20" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="E20" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G20" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H20" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I20" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J20" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="B21" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D21" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="E21" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G21" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H21" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I21" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J21" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="B22" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D22" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="E22" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G22" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H22" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I22" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J22" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="B23" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D23" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="E23" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G23" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H23" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I23" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J23" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="B24" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D24" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="E24" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F24" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G24" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H24" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I24" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J24" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="B25" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D25" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="E25" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F25" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G25" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H25" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I25" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J25" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="B26" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D26" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="E26" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F26" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G26" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H26" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I26" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J26" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="B27" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D27" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="E27" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F27" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G27" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H27" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I27" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J27" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>52</v>
+        <v>24</v>
       </c>
       <c r="B28" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D28" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="E28" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F28" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G28" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H28" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I28" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J28" t="s">
-        <v>62</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="B29" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D29" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="E29" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F29" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G29" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H29" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I29" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J29" t="s">
-        <v>62</v>
+        <v>25</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="B30" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D30" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="E30" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F30" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G30" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H30" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I30" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J30" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="B31" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D31" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="E31" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F31" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G31" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H31" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I31" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J31" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="B32" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D32" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="E32" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F32" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G32" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H32" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I32" t="s">
-        <v>13</v>
-      </c>
-      <c r="J32" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="B33" t="s">
-        <v>7</v>
-      </c>
-      <c r="D33" t="s">
-        <v>30</v>
-      </c>
-      <c r="E33" t="s">
-        <v>11</v>
-      </c>
-      <c r="F33" t="s">
-        <v>8</v>
-      </c>
-      <c r="G33" t="s">
-        <v>10</v>
-      </c>
-      <c r="H33" t="s">
-        <v>12</v>
-      </c>
-      <c r="I33" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="J33" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>57</v>
-      </c>
-      <c r="B34" t="s">
-        <v>7</v>
-      </c>
-      <c r="D34" t="s">
-        <v>30</v>
-      </c>
-      <c r="E34" t="s">
-        <v>11</v>
-      </c>
-      <c r="F34" t="s">
-        <v>8</v>
-      </c>
-      <c r="G34" t="s">
-        <v>10</v>
-      </c>
-      <c r="H34" t="s">
-        <v>12</v>
-      </c>
-      <c r="I34" t="s">
-        <v>13</v>
-      </c>
-      <c r="J34" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>58</v>
-      </c>
-      <c r="B35" t="s">
-        <v>7</v>
-      </c>
-      <c r="D35" t="s">
-        <v>30</v>
-      </c>
-      <c r="E35" t="s">
-        <v>11</v>
-      </c>
-      <c r="F35" t="s">
-        <v>8</v>
-      </c>
-      <c r="G35" t="s">
-        <v>10</v>
-      </c>
-      <c r="H35" t="s">
-        <v>12</v>
-      </c>
-      <c r="I35" t="s">
-        <v>13</v>
-      </c>
-      <c r="J35" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>59</v>
-      </c>
-      <c r="B36" t="s">
-        <v>7</v>
-      </c>
-      <c r="D36" t="s">
-        <v>30</v>
-      </c>
-      <c r="E36" t="s">
-        <v>11</v>
-      </c>
-      <c r="F36" t="s">
-        <v>8</v>
-      </c>
-      <c r="G36" t="s">
-        <v>10</v>
-      </c>
-      <c r="H36" t="s">
-        <v>12</v>
-      </c>
-      <c r="I36" t="s">
-        <v>13</v>
-      </c>
-      <c r="J36" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>60</v>
-      </c>
-      <c r="B37" t="s">
-        <v>6</v>
-      </c>
-      <c r="J37" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C345D6C-DF3E-47DC-B08A-E822CBA15E43}">
-  <dimension ref="A1:K6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="26.7109375" customWidth="1"/>
-    <col min="2" max="2" width="48.28515625" customWidth="1"/>
-    <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="30.28515625" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" t="s">
-        <v>11</v>
-      </c>
-      <c r="J2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I3" t="s">
-        <v>11</v>
-      </c>
-      <c r="J3" t="s">
-        <v>12</v>
-      </c>
-      <c r="K3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G4" t="s">
-        <v>9</v>
-      </c>
-      <c r="I4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I5" t="s">
-        <v>11</v>
-      </c>
-      <c r="J5" t="s">
-        <v>12</v>
-      </c>
-      <c r="K5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" t="s">
-        <v>3</v>
-      </c>
-      <c r="F6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6" t="s">
-        <v>10</v>
-      </c>
-      <c r="I6" t="s">
-        <v>11</v>
-      </c>
-      <c r="J6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3C5DDC6-63D8-46D9-AC4D-F73BC5AAF5EE}">
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="26.7109375" customWidth="1"/>
-    <col min="2" max="2" width="48.28515625" customWidth="1"/>
-    <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="30.28515625" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>